<commit_message>
feat(dataImport) : Tratamento dos dados finalizado e dados exportados para o banco
</commit_message>
<xml_diff>
--- a/Excel/fornecedores.xlsx
+++ b/Excel/fornecedores.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emanu\OneDrive\Área de Trabalho\Sistema Gerenciador de Fornecedores\Vendor Management System\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC42311-67FD-44A3-A881-F888991BEF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74C5961-E01B-4946-9DA1-9DC9E119F186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Empresas" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1214,26 +1219,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A8:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" customWidth="1"/>
-    <col min="10" max="10" width="54.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" customWidth="1"/>
+    <col min="10" max="10" width="54.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1265,7 +1270,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1294,7 +1299,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1326,7 +1331,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1355,7 +1360,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1387,7 +1392,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -1416,7 +1421,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -1448,7 +1453,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -1477,7 +1482,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>72</v>
       </c>
@@ -1509,7 +1514,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>81</v>
       </c>
@@ -1541,7 +1546,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>90</v>
       </c>
@@ -1570,7 +1575,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>97</v>
       </c>
@@ -1602,7 +1607,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>106</v>
       </c>
@@ -1631,7 +1636,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>115</v>
       </c>
@@ -1660,7 +1665,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>123</v>
       </c>
@@ -1689,7 +1694,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>131</v>
       </c>
@@ -1709,7 +1714,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>135</v>
       </c>
@@ -1738,7 +1743,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>143</v>
       </c>
@@ -1770,7 +1775,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>151</v>
       </c>
@@ -1799,7 +1804,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>157</v>
       </c>
@@ -1831,7 +1836,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>166</v>
       </c>
@@ -1860,7 +1865,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>174</v>
       </c>
@@ -1889,7 +1894,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>181</v>
       </c>
@@ -1905,7 +1910,7 @@
       <c r="E30" t="s">
         <v>184</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>185</v>
       </c>
       <c r="I30" t="s">
@@ -1915,7 +1920,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>187</v>
       </c>
@@ -1947,7 +1952,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>194</v>
       </c>
@@ -1973,7 +1978,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>202</v>
       </c>
@@ -2002,7 +2007,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>208</v>
       </c>
@@ -2031,7 +2036,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>214</v>
       </c>
@@ -2057,7 +2062,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>220</v>
       </c>
@@ -2086,7 +2091,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>227</v>
       </c>
@@ -2118,7 +2123,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>235</v>
       </c>
@@ -2147,7 +2152,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>241</v>
       </c>
@@ -2176,7 +2181,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>249</v>
       </c>
@@ -2205,7 +2210,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>255</v>
       </c>
@@ -2234,7 +2239,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>263</v>
       </c>
@@ -2250,7 +2255,7 @@
       <c r="E42" t="s">
         <v>266</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>267</v>
       </c>
       <c r="I42" t="s">
@@ -2260,7 +2265,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>269</v>
       </c>

</xml_diff>